<commit_message>
Mise à jour du mapping et correction des erreurs liées dans le ML et ressources FHIR d3b0e9201c582b7e8e6b81c5760539b0a154491e
</commit_message>
<xml_diff>
--- a/mappingCorps/ig/FRActLMCDAFHIR.xlsx
+++ b/mappingCorps/ig/FRActLMCDAFHIR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="87">
   <si>
     <t>Property</t>
   </si>
@@ -55,7 +55,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-16T14:59:20+00:00</t>
+    <t>2026-01-22T09:24:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>FRProcedureActDocument.recorder.extension:author</t>
-  </si>
-  <si>
-    <t>priorityCode</t>
   </si>
   <si>
     <t>FRProcedureActDocument.extension:priority</t>
@@ -1050,14 +1047,14 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -1070,7 +1067,7 @@
         <v>32</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="2"/>
     </row>
@@ -1083,7 +1080,7 @@
         <v>32</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2"/>
     </row>

</xml_diff>